<commit_message>
Blanked out file to make ready for deployment.
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10816"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10822"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdshowman/TechCheckout/TechCheck/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA06838-CF41-C24C-9BD7-FFB6320F2ACA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F72269E-8A15-6945-BB48-022A1A308901}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="440" windowWidth="26740" windowHeight="13560" xr2:uid="{F77DE8DF-4E79-2B4C-889A-59C6DF9866E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>AssetID</t>
   </si>
@@ -37,27 +37,6 @@
   </si>
   <si>
     <t>DateBorrowed</t>
-  </si>
-  <si>
-    <t>CB11</t>
-  </si>
-  <si>
-    <t>CB13</t>
-  </si>
-  <si>
-    <t>iPad</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>08/21/2018</t>
-  </si>
-  <si>
-    <t>Johnny Tsunami</t>
   </si>
 </sst>
 </file>
@@ -93,8 +72,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -410,16 +390,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88AFEB53-0063-674F-9FEB-7355638F0085}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="16384" width="10.83203125" style="1" collapsed="1"/>
@@ -440,46 +420,82 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>11111111</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>22222222</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>33333333</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>